<commit_message>
update mockup data to template
</commit_message>
<xml_diff>
--- a/data/online-dependency-open_template_v2.xlsx
+++ b/data/online-dependency-open_template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Source Code\Python\jupiter-service-inventory-importer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403F783D-E01D-4BF8-B949-F4621D632196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFEC922-D11F-455F-90F5-65C95C3D1F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-720" yWindow="4392" windowWidth="25920" windowHeight="13572" xr2:uid="{E9D40224-B996-4074-BAC3-1CED93BA3F06}"/>
+    <workbookView xWindow="2352" yWindow="3480" windowWidth="21336" windowHeight="13572" xr2:uid="{E9D40224-B996-4074-BAC3-1CED93BA3F06}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumer Template" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t>consumer_app_id</t>
   </si>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t>11, 18, 45</t>
+  </si>
+  <si>
+    <t>100_EBS_2651C71AAA9915B8F7044F388F8B5EF3</t>
+  </si>
+  <si>
+    <t>100_EBS_4EB46DD6C644398BBAC0A11CBC98846E</t>
+  </si>
+  <si>
+    <t>100_EBS_7D09E83A3C3A01CA5A65A5D6EB34E2F9</t>
+  </si>
+  <si>
+    <t>27_ST (SA)_555F96851410660A08713F0FC714B04E</t>
+  </si>
+  <si>
+    <t>654_ANYID_186347CE17A9F0D16651C0881111D5A3</t>
+  </si>
+  <si>
+    <t>100_EBS_A9F665AE5AF6848F54770E5DEF91B2A3</t>
   </si>
 </sst>
 </file>
@@ -1037,52 +1055,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768A2715-9E44-44E7-8F0B-336BABD4A3DA}">
-  <dimension ref="A1:BJ38"/>
+  <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BL9" sqref="BL9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="55" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.09765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.59765625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.09765625" style="4" customWidth="1"/>
-    <col min="10" max="11" width="20.09765625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="27.09765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="29.59765625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.08984375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="59.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.08984375" style="4" customWidth="1"/>
+    <col min="10" max="11" width="20.08984375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="27.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="29.6328125" style="4" customWidth="1"/>
     <col min="19" max="19" width="12" style="4" customWidth="1"/>
-    <col min="20" max="20" width="14.59765625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="13.3984375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="15.09765625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="15.59765625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="11.09765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.8984375" style="4" customWidth="1"/>
-    <col min="26" max="27" width="14.59765625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="14.8984375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="14.6328125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="13.36328125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.08984375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.6328125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="11.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.90625" style="4" customWidth="1"/>
+    <col min="26" max="27" width="14.6328125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="14.90625" style="4" customWidth="1"/>
     <col min="29" max="29" width="12" style="4" customWidth="1"/>
     <col min="30" max="30" width="12" style="2" customWidth="1"/>
     <col min="31" max="36" width="12" style="4" customWidth="1"/>
-    <col min="37" max="37" width="31.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="42.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="40.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="41.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="51" width="12.09765625" style="4" customWidth="1"/>
-    <col min="52" max="52" width="18.296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="26.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="31.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="29.59765625" style="4" customWidth="1"/>
-    <col min="59" max="59" width="21.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="27.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="42.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="40.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="41.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="51" width="12.08984375" style="4" customWidth="1"/>
+    <col min="52" max="52" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="26.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="31.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="29.6328125" style="4" customWidth="1"/>
+    <col min="59" max="59" width="21.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="18.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="27.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="25" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1718,6 +1736,62 @@
         <v>94</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I2:K839">
     <cfRule type="expression" dxfId="20" priority="5">

</xml_diff>